<commit_message>
Initialized set of Requirements
</commit_message>
<xml_diff>
--- a/requirements/REQUIREMENTS_241119.xlsx
+++ b/requirements/REQUIREMENTS_241119.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtramontata\Desktop\PeSoS\2019_assignment2_unimib_tutoring_assistant\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5987D7A0-E395-413B-8786-D6D88D22AD65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72B5E54-188C-4208-B08B-39614575C08D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>ID_REQUIREMENT</t>
   </si>
   <si>
     <t>DESCRIPTION_REQUIREMENT</t>
+  </si>
+  <si>
+    <t>Integration with OS Calendar</t>
+  </si>
+  <si>
+    <t>Usage of real personal data</t>
+  </si>
+  <si>
+    <t>Integration with a geolocalization provider</t>
+  </si>
+  <si>
+    <t>Implementation of a built-in chat system</t>
+  </si>
+  <si>
+    <t>Implementation of a complex Search Functionality</t>
+  </si>
+  <si>
+    <t>Implementation of a complete rating system</t>
+  </si>
+  <si>
+    <t>Implementation of a workflow for "User Profile" functionalities</t>
   </si>
 </sst>
 </file>
@@ -348,16 +369,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -368,6 +389,77 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Result of the interview (last question WIP)
</commit_message>
<xml_diff>
--- a/requirements/REQUIREMENTS_241119.xlsx
+++ b/requirements/REQUIREMENTS_241119.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtramontata\Desktop\PeSoS\2019_assignment2_unimib_tutoring_assistant\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E977AF8A-F0AE-4341-9DC0-C0C1ED300D42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959A6EEE-F480-4897-8B47-C64D07BE8229}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ID_REQUIREMENT</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>Implementation of a workflow for "User Profile" functionalities</t>
+  </si>
+  <si>
+    <t>Implementation of a complex form to publish lessons timetable</t>
+  </si>
+  <si>
+    <t>Implementation of a workflow allowing to save "connections" with other people</t>
+  </si>
+  <si>
+    <t>Implementation of the Search filter by teacher's name</t>
   </si>
 </sst>
 </file>
@@ -369,19 +378,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,7 +398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -397,7 +406,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -405,7 +414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -413,7 +422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -421,7 +430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -429,7 +438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -437,7 +446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -445,9 +454,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final adjustments to Requirements
</commit_message>
<xml_diff>
--- a/requirements/REQUIREMENTS_241119.xlsx
+++ b/requirements/REQUIREMENTS_241119.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtramontata\Desktop\PeSoS\2019_assignment2_unimib_tutoring_assistant\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCF036B-C0C7-46F6-A1D6-5A0FEA88874A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB4ABD8-3E14-4655-80B7-EE7253A71076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ID_REQUIREMENT</t>
   </si>
   <si>
-    <t>DESCRIPTION_REQUIREMENT</t>
-  </si>
-  <si>
     <t>Integration with OS Calendar</t>
   </si>
   <si>
@@ -60,7 +57,43 @@
     <t>Implementation of a workflow allowing to save "connections" with other people</t>
   </si>
   <si>
-    <t>Implementation of the Search filter by teacher's name</t>
+    <t>REQUIREMENT_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>REQUIREMENT_NAME</t>
+  </si>
+  <si>
+    <t>The users should be able to compile their own "User Profile" form, providing a chosen set of information.
+Every  user should also be able to consult other users' "User Profile".</t>
+  </si>
+  <si>
+    <t>A user searching for a private lesson should be able to, at least:
+1. Search for a teacher directly by name or email;
+2. Filter the research by field of interest;
+3. Sort by price, feedback of other users, map location.</t>
+  </si>
+  <si>
+    <t>The users should be able to start an instant messaging communication with other users.
+The users should also be able to access their chats in an easy and structured manner.</t>
+  </si>
+  <si>
+    <t>The teachers should be able to set an indicative geographical location for their private lessons with the help of a geolocalization provider.
+The students should be able to use such geolocalization provider to access the details of the geographical location set by the teacher.</t>
+  </si>
+  <si>
+    <t>The users should be encouraged to use their personal data by connecting their account with a Social Network Active Directory. Facebook is the preferred choice for this.</t>
+  </si>
+  <si>
+    <t>The Mobile App should use OS APIs to connect with the user's default Calendar App to notify them about upcoming private lessons.</t>
+  </si>
+  <si>
+    <t>Both teachers and students should be able to give a public feedback about the persons they are interacting with. The users should be given the possibility to send a feedback after a certain time after a scheduled private lessons and they should be able to, at least, assing an overall rating and a description.</t>
+  </si>
+  <si>
+    <t>The users should be able to flag other users as "favorite": this could allow the users to have their favorites marked in every UI of the Mobile App.</t>
+  </si>
+  <si>
+    <t>For every published private lesson offer, a teacher should be able to define and publish a complete timetable through the help of a form.</t>
   </si>
 </sst>
 </file>
@@ -68,9 +101,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="000"/>
+    <numFmt numFmtId="164" formatCode="000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,16 +111,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -95,13 +142,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,108 +454,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="C9" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="C10" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>